<commit_message>
fix schema & no duplicate nesting count
</commit_message>
<xml_diff>
--- a/Calculs a la mano.xlsx
+++ b/Calculs a la mano.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7009dbc6f400b33/Documents/Travail/ESILV/S9/Big Data Structure/big_data_structure/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\A5_BigDataStructure\big_data_structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="683" documentId="8_{C6A58793-CBB7-451A-85AC-19D981C38815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C6567A4-9D89-4A11-96ED-B47301FA3DAF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46ADAE8-77DF-485F-B59C-4BA8F8ADEC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{EC06A178-667E-4206-997B-DB84C90162B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EC06A178-667E-4206-997B-DB84C90162B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -485,7 +485,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -804,10 +804,10 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="3" width="15.7109375" customWidth="1"/>
@@ -1833,7 +1833,7 @@
         <f>SUM(Table1[[#This Row],[Int/num]:[LongString]]) - 6 + Table1[[#This Row],[avg array length]]*(SUM(Table1[[#This Row],[array int]:[array date]]))</f>
         <v>240011</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="1">
         <f>Table1[[#This Row],[Int/num]]*$B$2 + Table1[[#This Row],[String]]*$C$2 + Table1[[#This Row],[Date]]*$D$2 + Table1[[#This Row],[LongString]]*$E$2 + Table1[[#This Row],[array int]]*Table1[[#This Row],[avg array length]]*$G$2 + Table1[[#This Row],[array string]]*Table1[[#This Row],[avg array length]]*$H$2 + Table1[[#This Row],[array longstring]]*Table1[[#This Row],[avg array length]]*$I$2 + Table1[[#This Row],[array date]]*Table1[[#This Row],[avg array length]]*$J$2 + Table1[[#This Row],[keys]]*$K$2</f>
         <v>13441108</v>
       </c>

</xml_diff>